<commit_message>
al,am,ap,ba,ce,df ok agora no es
</commit_message>
<xml_diff>
--- a/dados_brutos/Hemoprod_AM.xlsx
+++ b/dados_brutos/Hemoprod_AM.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Hemoprod\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\STTP\hemodata\hemodata\dados_brutos\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FA8ED37-C1A8-433A-AE81-31B20ED0DAE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12180"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HEMOPROD - AMAZONAS" sheetId="1" r:id="rId1"/>
@@ -1120,7 +1121,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1209,9 +1210,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1249,9 +1250,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1286,7 +1287,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1321,7 +1322,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1494,12 +1495,284 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:JJ33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="94.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="36.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="118.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="35.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="39.140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="130.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="52.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="81.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="83.140625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="80.42578125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="81.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="79.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="80.85546875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="65.5703125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="67.140625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="63.42578125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="64.85546875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="64.140625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="65.5703125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="66.42578125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="68" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="65.7109375" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="67.28515625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="70.7109375" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="72.28515625" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="67.28515625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="68.7109375" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="70.140625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="71.7109375" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="83.85546875" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="83" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="78.85546875" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="88" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="87.140625" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="83" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="87.140625" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="86.42578125" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="82.28515625" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="86.85546875" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="86.140625" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="82" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="107.5703125" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="106.85546875" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="102.7109375" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="89.5703125" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="88.85546875" bestFit="1" customWidth="1"/>
+    <col min="65" max="66" width="84.7109375" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="84" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="79.85546875" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="93.140625" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="92.42578125" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="88.28515625" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="83.7109375" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="82.85546875" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="78.7109375" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="82.7109375" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="82" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="77.85546875" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="41.85546875" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="64.85546875" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="49.140625" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="51.5703125" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="27" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="104" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="105.5703125" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="90.85546875" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="92.42578125" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="93.140625" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="94.5703125" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="105.5703125" bestFit="1" customWidth="1"/>
+    <col min="92" max="93" width="107" bestFit="1" customWidth="1"/>
+    <col min="94" max="94" width="108.5703125" bestFit="1" customWidth="1"/>
+    <col min="95" max="95" width="97.28515625" bestFit="1" customWidth="1"/>
+    <col min="96" max="96" width="98.7109375" bestFit="1" customWidth="1"/>
+    <col min="97" max="97" width="97" bestFit="1" customWidth="1"/>
+    <col min="98" max="98" width="98.42578125" bestFit="1" customWidth="1"/>
+    <col min="99" max="99" width="94.5703125" bestFit="1" customWidth="1"/>
+    <col min="100" max="100" width="96.140625" bestFit="1" customWidth="1"/>
+    <col min="101" max="101" width="103.7109375" bestFit="1" customWidth="1"/>
+    <col min="102" max="102" width="105.28515625" bestFit="1" customWidth="1"/>
+    <col min="103" max="103" width="103.7109375" bestFit="1" customWidth="1"/>
+    <col min="104" max="104" width="105.28515625" bestFit="1" customWidth="1"/>
+    <col min="105" max="105" width="103.140625" bestFit="1" customWidth="1"/>
+    <col min="106" max="106" width="104.7109375" bestFit="1" customWidth="1"/>
+    <col min="107" max="107" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="108" max="108" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="109" max="109" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="110" max="110" width="35.140625" bestFit="1" customWidth="1"/>
+    <col min="111" max="111" width="34.85546875" bestFit="1" customWidth="1"/>
+    <col min="112" max="112" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="113" max="113" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="114" max="114" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="115" max="115" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="116" max="116" width="35" bestFit="1" customWidth="1"/>
+    <col min="117" max="117" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="118" max="118" width="34.85546875" bestFit="1" customWidth="1"/>
+    <col min="119" max="119" width="34.5703125" bestFit="1" customWidth="1"/>
+    <col min="120" max="120" width="36.140625" bestFit="1" customWidth="1"/>
+    <col min="121" max="121" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="122" max="122" width="35.140625" bestFit="1" customWidth="1"/>
+    <col min="123" max="123" width="37.140625" bestFit="1" customWidth="1"/>
+    <col min="124" max="124" width="38.85546875" bestFit="1" customWidth="1"/>
+    <col min="125" max="125" width="67.5703125" bestFit="1" customWidth="1"/>
+    <col min="126" max="126" width="69.140625" bestFit="1" customWidth="1"/>
+    <col min="127" max="127" width="43.42578125" bestFit="1" customWidth="1"/>
+    <col min="128" max="128" width="45" bestFit="1" customWidth="1"/>
+    <col min="129" max="129" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="130" max="130" width="45.28515625" bestFit="1" customWidth="1"/>
+    <col min="131" max="131" width="53" bestFit="1" customWidth="1"/>
+    <col min="132" max="132" width="57.42578125" bestFit="1" customWidth="1"/>
+    <col min="133" max="133" width="83.5703125" bestFit="1" customWidth="1"/>
+    <col min="134" max="134" width="84.85546875" bestFit="1" customWidth="1"/>
+    <col min="135" max="135" width="27" bestFit="1" customWidth="1"/>
+    <col min="136" max="136" width="64.7109375" bestFit="1" customWidth="1"/>
+    <col min="137" max="137" width="64" bestFit="1" customWidth="1"/>
+    <col min="138" max="138" width="64.7109375" bestFit="1" customWidth="1"/>
+    <col min="139" max="139" width="76.42578125" bestFit="1" customWidth="1"/>
+    <col min="140" max="140" width="75.7109375" bestFit="1" customWidth="1"/>
+    <col min="141" max="141" width="76.42578125" bestFit="1" customWidth="1"/>
+    <col min="142" max="142" width="67.140625" bestFit="1" customWidth="1"/>
+    <col min="143" max="143" width="66.28515625" bestFit="1" customWidth="1"/>
+    <col min="144" max="144" width="67.140625" bestFit="1" customWidth="1"/>
+    <col min="145" max="145" width="77" bestFit="1" customWidth="1"/>
+    <col min="146" max="146" width="76.28515625" bestFit="1" customWidth="1"/>
+    <col min="147" max="147" width="77" bestFit="1" customWidth="1"/>
+    <col min="148" max="148" width="90.85546875" bestFit="1" customWidth="1"/>
+    <col min="149" max="149" width="90.140625" bestFit="1" customWidth="1"/>
+    <col min="150" max="150" width="90.85546875" bestFit="1" customWidth="1"/>
+    <col min="151" max="151" width="77.28515625" bestFit="1" customWidth="1"/>
+    <col min="152" max="152" width="76.5703125" bestFit="1" customWidth="1"/>
+    <col min="153" max="153" width="77.28515625" bestFit="1" customWidth="1"/>
+    <col min="154" max="154" width="87.85546875" bestFit="1" customWidth="1"/>
+    <col min="155" max="155" width="87" bestFit="1" customWidth="1"/>
+    <col min="156" max="156" width="87.85546875" bestFit="1" customWidth="1"/>
+    <col min="157" max="157" width="77.85546875" bestFit="1" customWidth="1"/>
+    <col min="158" max="158" width="77.140625" bestFit="1" customWidth="1"/>
+    <col min="159" max="159" width="77.85546875" bestFit="1" customWidth="1"/>
+    <col min="160" max="160" width="67.5703125" bestFit="1" customWidth="1"/>
+    <col min="161" max="161" width="66.7109375" bestFit="1" customWidth="1"/>
+    <col min="162" max="162" width="67.5703125" bestFit="1" customWidth="1"/>
+    <col min="163" max="163" width="91.140625" bestFit="1" customWidth="1"/>
+    <col min="164" max="164" width="90.42578125" bestFit="1" customWidth="1"/>
+    <col min="165" max="165" width="91.140625" bestFit="1" customWidth="1"/>
+    <col min="166" max="166" width="48" bestFit="1" customWidth="1"/>
+    <col min="167" max="167" width="36" bestFit="1" customWidth="1"/>
+    <col min="168" max="168" width="41.85546875" bestFit="1" customWidth="1"/>
+    <col min="169" max="169" width="59.7109375" bestFit="1" customWidth="1"/>
+    <col min="170" max="170" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="171" max="171" width="53.5703125" bestFit="1" customWidth="1"/>
+    <col min="172" max="172" width="50.42578125" bestFit="1" customWidth="1"/>
+    <col min="173" max="173" width="38.42578125" bestFit="1" customWidth="1"/>
+    <col min="174" max="174" width="44.28515625" bestFit="1" customWidth="1"/>
+    <col min="175" max="175" width="60.28515625" bestFit="1" customWidth="1"/>
+    <col min="176" max="176" width="48.28515625" bestFit="1" customWidth="1"/>
+    <col min="177" max="177" width="54.140625" bestFit="1" customWidth="1"/>
+    <col min="178" max="178" width="74.140625" bestFit="1" customWidth="1"/>
+    <col min="179" max="179" width="62.140625" bestFit="1" customWidth="1"/>
+    <col min="180" max="180" width="68.140625" bestFit="1" customWidth="1"/>
+    <col min="181" max="181" width="60.5703125" bestFit="1" customWidth="1"/>
+    <col min="182" max="182" width="48.5703125" bestFit="1" customWidth="1"/>
+    <col min="183" max="183" width="54.5703125" bestFit="1" customWidth="1"/>
+    <col min="184" max="184" width="71.140625" bestFit="1" customWidth="1"/>
+    <col min="185" max="185" width="59.140625" bestFit="1" customWidth="1"/>
+    <col min="186" max="186" width="65" bestFit="1" customWidth="1"/>
+    <col min="187" max="187" width="61.140625" bestFit="1" customWidth="1"/>
+    <col min="188" max="188" width="49.140625" bestFit="1" customWidth="1"/>
+    <col min="189" max="189" width="55.140625" bestFit="1" customWidth="1"/>
+    <col min="190" max="190" width="50.85546875" bestFit="1" customWidth="1"/>
+    <col min="191" max="191" width="38.85546875" bestFit="1" customWidth="1"/>
+    <col min="192" max="192" width="44.7109375" bestFit="1" customWidth="1"/>
+    <col min="193" max="193" width="74.42578125" bestFit="1" customWidth="1"/>
+    <col min="194" max="194" width="62.42578125" bestFit="1" customWidth="1"/>
+    <col min="195" max="195" width="68.42578125" bestFit="1" customWidth="1"/>
+    <col min="196" max="196" width="43.42578125" bestFit="1" customWidth="1"/>
+    <col min="197" max="197" width="40.7109375" bestFit="1" customWidth="1"/>
+    <col min="198" max="198" width="36" bestFit="1" customWidth="1"/>
+    <col min="199" max="199" width="55.140625" bestFit="1" customWidth="1"/>
+    <col min="200" max="200" width="52.42578125" bestFit="1" customWidth="1"/>
+    <col min="201" max="201" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="202" max="202" width="45.7109375" bestFit="1" customWidth="1"/>
+    <col min="203" max="203" width="43.140625" bestFit="1" customWidth="1"/>
+    <col min="204" max="204" width="38.42578125" bestFit="1" customWidth="1"/>
+    <col min="205" max="205" width="55.7109375" bestFit="1" customWidth="1"/>
+    <col min="206" max="206" width="53" bestFit="1" customWidth="1"/>
+    <col min="207" max="207" width="48.28515625" bestFit="1" customWidth="1"/>
+    <col min="208" max="208" width="69.5703125" bestFit="1" customWidth="1"/>
+    <col min="209" max="209" width="67" bestFit="1" customWidth="1"/>
+    <col min="210" max="210" width="62.140625" bestFit="1" customWidth="1"/>
+    <col min="211" max="211" width="56" bestFit="1" customWidth="1"/>
+    <col min="212" max="212" width="53.28515625" bestFit="1" customWidth="1"/>
+    <col min="213" max="213" width="48.5703125" bestFit="1" customWidth="1"/>
+    <col min="214" max="214" width="66.42578125" bestFit="1" customWidth="1"/>
+    <col min="215" max="215" width="63.85546875" bestFit="1" customWidth="1"/>
+    <col min="216" max="216" width="59.140625" bestFit="1" customWidth="1"/>
+    <col min="217" max="217" width="56.5703125" bestFit="1" customWidth="1"/>
+    <col min="218" max="218" width="53.85546875" bestFit="1" customWidth="1"/>
+    <col min="219" max="219" width="49.140625" bestFit="1" customWidth="1"/>
+    <col min="220" max="220" width="46.28515625" bestFit="1" customWidth="1"/>
+    <col min="221" max="221" width="43.5703125" bestFit="1" customWidth="1"/>
+    <col min="222" max="222" width="38.85546875" bestFit="1" customWidth="1"/>
+    <col min="223" max="223" width="69.85546875" bestFit="1" customWidth="1"/>
+    <col min="224" max="224" width="67.28515625" bestFit="1" customWidth="1"/>
+    <col min="225" max="225" width="62.42578125" bestFit="1" customWidth="1"/>
+    <col min="226" max="226" width="80" bestFit="1" customWidth="1"/>
+    <col min="227" max="227" width="80.140625" bestFit="1" customWidth="1"/>
+    <col min="228" max="228" width="57.140625" bestFit="1" customWidth="1"/>
+    <col min="229" max="229" width="91.5703125" bestFit="1" customWidth="1"/>
+    <col min="230" max="230" width="91.85546875" bestFit="1" customWidth="1"/>
+    <col min="231" max="231" width="68.85546875" bestFit="1" customWidth="1"/>
+    <col min="232" max="232" width="82.28515625" bestFit="1" customWidth="1"/>
+    <col min="233" max="233" width="82.42578125" bestFit="1" customWidth="1"/>
+    <col min="234" max="234" width="59.5703125" bestFit="1" customWidth="1"/>
+    <col min="235" max="235" width="92.28515625" bestFit="1" customWidth="1"/>
+    <col min="236" max="236" width="92.42578125" bestFit="1" customWidth="1"/>
+    <col min="237" max="237" width="69.42578125" bestFit="1" customWidth="1"/>
+    <col min="238" max="238" width="106.140625" bestFit="1" customWidth="1"/>
+    <col min="239" max="239" width="106.28515625" bestFit="1" customWidth="1"/>
+    <col min="240" max="240" width="83.28515625" bestFit="1" customWidth="1"/>
+    <col min="241" max="241" width="92.5703125" bestFit="1" customWidth="1"/>
+    <col min="242" max="242" width="92.7109375" bestFit="1" customWidth="1"/>
+    <col min="243" max="243" width="69.7109375" bestFit="1" customWidth="1"/>
+    <col min="244" max="244" width="103" bestFit="1" customWidth="1"/>
+    <col min="245" max="245" width="103.140625" bestFit="1" customWidth="1"/>
+    <col min="246" max="246" width="80.28515625" bestFit="1" customWidth="1"/>
+    <col min="247" max="247" width="93.140625" bestFit="1" customWidth="1"/>
+    <col min="248" max="248" width="93.28515625" bestFit="1" customWidth="1"/>
+    <col min="249" max="249" width="70.28515625" bestFit="1" customWidth="1"/>
+    <col min="250" max="250" width="82.7109375" bestFit="1" customWidth="1"/>
+    <col min="251" max="251" width="82.85546875" bestFit="1" customWidth="1"/>
+    <col min="252" max="252" width="60" bestFit="1" customWidth="1"/>
+    <col min="253" max="253" width="106.42578125" bestFit="1" customWidth="1"/>
+    <col min="254" max="254" width="106.5703125" bestFit="1" customWidth="1"/>
+    <col min="255" max="255" width="83.7109375" bestFit="1" customWidth="1"/>
+    <col min="256" max="256" width="68.7109375" bestFit="1" customWidth="1"/>
+    <col min="257" max="257" width="69.7109375" bestFit="1" customWidth="1"/>
+    <col min="258" max="258" width="98.85546875" bestFit="1" customWidth="1"/>
+    <col min="259" max="259" width="98.7109375" bestFit="1" customWidth="1"/>
+    <col min="260" max="260" width="84.28515625" bestFit="1" customWidth="1"/>
+    <col min="261" max="261" width="51.7109375" bestFit="1" customWidth="1"/>
+    <col min="262" max="262" width="42.140625" bestFit="1" customWidth="1"/>
+    <col min="263" max="263" width="39.5703125" bestFit="1" customWidth="1"/>
+    <col min="264" max="264" width="42.5703125" bestFit="1" customWidth="1"/>
+    <col min="265" max="265" width="46.7109375" bestFit="1" customWidth="1"/>
+    <col min="266" max="266" width="44.28515625" bestFit="1" customWidth="1"/>
+    <col min="267" max="267" width="39.28515625" bestFit="1" customWidth="1"/>
+    <col min="268" max="268" width="73.5703125" bestFit="1" customWidth="1"/>
+    <col min="269" max="269" width="64.5703125" bestFit="1" customWidth="1"/>
+    <col min="270" max="270" width="27" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:270" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -27402,28 +27675,28 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J2" r:id="rId1"/>
-    <hyperlink ref="J3" r:id="rId2"/>
-    <hyperlink ref="J4" r:id="rId3"/>
-    <hyperlink ref="J5" r:id="rId4"/>
-    <hyperlink ref="J6" r:id="rId5"/>
-    <hyperlink ref="J7" r:id="rId6"/>
-    <hyperlink ref="J8" r:id="rId7"/>
-    <hyperlink ref="J9" r:id="rId8"/>
-    <hyperlink ref="J10" r:id="rId9"/>
-    <hyperlink ref="J11" r:id="rId10"/>
-    <hyperlink ref="J12" r:id="rId11"/>
-    <hyperlink ref="J13" r:id="rId12"/>
-    <hyperlink ref="J16" r:id="rId13"/>
-    <hyperlink ref="J17" r:id="rId14"/>
-    <hyperlink ref="J18" r:id="rId15"/>
-    <hyperlink ref="J19" r:id="rId16"/>
-    <hyperlink ref="J20" r:id="rId17"/>
-    <hyperlink ref="J21" r:id="rId18"/>
-    <hyperlink ref="J22" r:id="rId19"/>
-    <hyperlink ref="J23" r:id="rId20"/>
-    <hyperlink ref="J27" r:id="rId21"/>
-    <hyperlink ref="J28" r:id="rId22"/>
+    <hyperlink ref="J2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="J3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="J4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="J5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="J6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="J7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="J8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="J9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="J10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="J11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="J12" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="J13" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="J16" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="J17" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="J18" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="J19" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="J20" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="J21" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="J22" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="J23" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="J27" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="J28" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -27607,18 +27880,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -27641,14 +27914,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3357F1D3-ED77-4A95-B393-F8A8BFAD9F12}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F80B05BB-ADCD-4286-851F-614AAA438C5B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="21ad56ba-f6ad-42d5-a412-f8823c1e07e0"/>
@@ -27663,4 +27928,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3357F1D3-ED77-4A95-B393-F8A8BFAD9F12}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>